<commit_message>
update screen + handle merge class
</commit_message>
<xml_diff>
--- a/Database/Data_20150722/Rooms.xlsx
+++ b/Database/Data_20150722/Rooms.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
   <si>
     <t>DS phòng</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>KN</t>
+  </si>
+  <si>
+    <t>HB/202R</t>
+  </si>
+  <si>
+    <t>LAB101, LAB211</t>
+  </si>
+  <si>
+    <t>GDG401, WMT201, DRA301, GDS301, CAA201, PST201, AFA201, GDF101, HOA101, DRF201, VCM201, DRS101, DGT101, PST201, DRP101, VNC101</t>
   </si>
 </sst>
 </file>
@@ -609,15 +618,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1327,7 +1336,9 @@
       <c r="C48" s="2">
         <v>30</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>57</v>
       </c>
@@ -1356,7 +1367,27 @@
       <c r="C50" s="2">
         <v>30</v>
       </c>
+      <c r="D50" t="s">
+        <v>62</v>
+      </c>
       <c r="E50" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>